<commit_message>
If else if else
</commit_message>
<xml_diff>
--- a/1.nen-tang-lap-trinh-java/4.Phat-bieu-dieu-kien.xlsx
+++ b/1.nen-tang-lap-trinh-java/4.Phat-bieu-dieu-kien.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\java\1.nen-tang-lap-trinh-java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60FCA612-98ED-4B43-B721-51066BC802E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FF0BC9-3A7E-4ADF-B12D-FEB4F78D48FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30405" yWindow="1050" windowWidth="25890" windowHeight="13545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30405" yWindow="1050" windowWidth="25890" windowHeight="13545" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="If" sheetId="1" r:id="rId1"/>
     <sheet name="If else" sheetId="2" r:id="rId2"/>
+    <sheet name="If else if else" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="90">
   <si>
     <t>java_training</t>
     <phoneticPr fontId="1"/>
@@ -399,12 +400,280 @@
     </r>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t xml:space="preserve">// 003 IF ELSE IF ELSE - Dạng 02 </t>
+  </si>
+  <si>
+    <t>public static void main007(String[] args) {</t>
+  </si>
+  <si>
+    <t>= -1;</t>
+  </si>
+  <si>
+    <t>//</t>
+  </si>
+  <si>
+    <t>n &gt;= 0 n%2==0</t>
+  </si>
+  <si>
+    <r>
+      <t>=&gt; n nguyên d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ươ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ng chẵn</t>
+    </r>
+  </si>
+  <si>
+    <t>n &gt;= 0 n%2==1</t>
+  </si>
+  <si>
+    <r>
+      <t>=&gt; n nguyên d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ươ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ng lẻ</t>
+    </r>
+  </si>
+  <si>
+    <t>n &lt; 0 n%2==0</t>
+  </si>
+  <si>
+    <t>=&gt; n nguyên âm chẵn</t>
+  </si>
+  <si>
+    <t>n &lt; 0 n%2==1</t>
+  </si>
+  <si>
+    <t>=&gt; n nguyên âm lẻ</t>
+  </si>
+  <si>
+    <t>if(number &gt;= 0 &amp;&amp; number %2 == 0){</t>
+  </si>
+  <si>
+    <t>result</t>
+  </si>
+  <si>
+    <r>
+      <t>= "nguyên d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ươ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ng chẵn";</t>
+    </r>
+  </si>
+  <si>
+    <t>} else if (number &gt;= 0 &amp;&amp; number %2 == 1){</t>
+  </si>
+  <si>
+    <r>
+      <t>= "nguyên d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ươ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ng lẻ";</t>
+    </r>
+  </si>
+  <si>
+    <t>} else if (number &lt; 0 &amp;&amp; number %2 == 0){</t>
+  </si>
+  <si>
+    <t>= "nguyên âm chẳn";</t>
+  </si>
+  <si>
+    <t>= "nguyên âm lẻ";</t>
+  </si>
+  <si>
+    <t xml:space="preserve">// 003 IF ELSE IF ELSE - Dạng 01 </t>
+  </si>
+  <si>
+    <t>public static void main006(String[] args) {</t>
+  </si>
+  <si>
+    <t>= 0;</t>
+  </si>
+  <si>
+    <t>if(number == 0) {</t>
+  </si>
+  <si>
+    <t>System.out.println("Số không");</t>
+  </si>
+  <si>
+    <t>}else if (number % 2 == 1){</t>
+  </si>
+  <si>
+    <t>}else{</t>
+  </si>
+  <si>
+    <t>System.out.println("Số chẵn");</t>
+  </si>
+  <si>
+    <t>// 002 IF ELSE</t>
+  </si>
+  <si>
+    <t>public static void main005(String[] args) {</t>
+  </si>
+  <si>
+    <t>int number	= 9;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>String str1	= "d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>ươ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ng";</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>String str2	= "ch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>ẵ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n";</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>if(number &lt; 0) 		str1 = "âm";</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>if(number %2 == 1) 	str2 = "l</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>ẻ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>";</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>System.out.println("nguyên " + str1 + " " + str2);</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -447,6 +716,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Yu Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="3">
@@ -555,7 +838,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -568,6 +851,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -716,6 +1001,99 @@
         <a:xfrm>
           <a:off x="790575" y="17002125"/>
           <a:ext cx="14028571" cy="5136508"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>353850</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>27365</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="図 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C8E7098-6DF8-960D-D01E-8D3B6D5C4053}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="809625" y="25095200"/>
+          <a:ext cx="14000000" cy="9682540"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>284825</xdr:colOff>
+      <xdr:row>173</xdr:row>
+      <xdr:rowOff>85215</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="図 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F52D145C-4097-AA2B-3CFC-F07B5CE7EF93}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="771525" y="35556825"/>
+          <a:ext cx="7400000" cy="4076190"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1610,8 +1988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BAB64A3-05E9-44CB-ACF2-846FFA30559A}">
   <dimension ref="B3:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="P106" sqref="P106"/>
+    <sheetView topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -2211,4 +2589,1532 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{887998C6-8081-42DF-AB4D-673412279D40}">
+  <dimension ref="B3:M174"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="Q167" sqref="Q167"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetData>
+    <row r="3" spans="2:9">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="2:9">
+      <c r="B4" s="4"/>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="2:9">
+      <c r="B5" s="4"/>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="2:9">
+      <c r="B6" s="4"/>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="2:9">
+      <c r="B7" s="4"/>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="B8" s="4"/>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="2:9">
+      <c r="B9" s="4"/>
+      <c r="E9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9">
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="9"/>
+    </row>
+    <row r="13" spans="2:9">
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9">
+      <c r="B14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="2:9">
+      <c r="B15" s="4"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="5"/>
+    </row>
+    <row r="16" spans="2:9">
+      <c r="B16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="5"/>
+    </row>
+    <row r="17" spans="2:9">
+      <c r="B17" s="4"/>
+      <c r="C17" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="5"/>
+    </row>
+    <row r="18" spans="2:9">
+      <c r="B18" s="4"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="5"/>
+    </row>
+    <row r="19" spans="2:9">
+      <c r="B19" s="4"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="5"/>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="B20" s="4"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="2:9">
+      <c r="B21" s="4"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="5"/>
+    </row>
+    <row r="22" spans="2:9">
+      <c r="B22" s="4"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="5"/>
+    </row>
+    <row r="23" spans="2:9">
+      <c r="B23" s="4"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="5"/>
+    </row>
+    <row r="24" spans="2:9">
+      <c r="B24" s="4"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="5"/>
+    </row>
+    <row r="25" spans="2:9">
+      <c r="B25" s="4"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="5"/>
+    </row>
+    <row r="26" spans="2:9">
+      <c r="B26" s="4"/>
+      <c r="C26" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="5"/>
+    </row>
+    <row r="27" spans="2:9">
+      <c r="B27" s="4"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="5"/>
+    </row>
+    <row r="28" spans="2:9">
+      <c r="B28" s="4"/>
+      <c r="C28" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="5"/>
+    </row>
+    <row r="29" spans="2:9">
+      <c r="B29" s="4"/>
+      <c r="C29" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="5"/>
+    </row>
+    <row r="30" spans="2:9">
+      <c r="B30" s="4"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="5"/>
+    </row>
+    <row r="31" spans="2:9">
+      <c r="B31" s="4"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="5"/>
+    </row>
+    <row r="32" spans="2:9">
+      <c r="B32" s="4"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="5"/>
+    </row>
+    <row r="33" spans="2:9">
+      <c r="B33" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="5"/>
+    </row>
+    <row r="34" spans="2:9">
+      <c r="B34" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="5"/>
+    </row>
+    <row r="35" spans="2:9">
+      <c r="B35" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="5"/>
+    </row>
+    <row r="36" spans="2:9">
+      <c r="B36" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="5"/>
+    </row>
+    <row r="37" spans="2:9">
+      <c r="B37" s="4"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="5"/>
+    </row>
+    <row r="38" spans="2:9">
+      <c r="B38" s="4"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="5"/>
+    </row>
+    <row r="39" spans="2:9">
+      <c r="B39" s="4"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="5"/>
+    </row>
+    <row r="40" spans="2:9">
+      <c r="B40" s="4"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="5"/>
+    </row>
+    <row r="41" spans="2:9">
+      <c r="B41" s="4"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F41" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="5"/>
+    </row>
+    <row r="42" spans="2:9">
+      <c r="B42" s="4"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="5"/>
+    </row>
+    <row r="43" spans="2:9">
+      <c r="B43" s="4"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F43" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="G43" s="12"/>
+      <c r="H43" s="12"/>
+      <c r="I43" s="5"/>
+    </row>
+    <row r="44" spans="2:9">
+      <c r="B44" s="4"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="5"/>
+    </row>
+    <row r="45" spans="2:9">
+      <c r="B45" s="4"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F45" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="5"/>
+    </row>
+    <row r="46" spans="2:9">
+      <c r="B46" s="4"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="5"/>
+    </row>
+    <row r="47" spans="2:9">
+      <c r="B47" s="4"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="12"/>
+      <c r="I47" s="5"/>
+    </row>
+    <row r="48" spans="2:9">
+      <c r="B48" s="4"/>
+      <c r="C48" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="12"/>
+      <c r="I48" s="5"/>
+    </row>
+    <row r="49" spans="2:9">
+      <c r="B49" s="4"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+      <c r="H49" s="12"/>
+      <c r="I49" s="5"/>
+    </row>
+    <row r="50" spans="2:9">
+      <c r="B50" s="4"/>
+      <c r="C50" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="12"/>
+      <c r="H50" s="12"/>
+      <c r="I50" s="5"/>
+    </row>
+    <row r="51" spans="2:9">
+      <c r="B51" s="4"/>
+      <c r="C51" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="12"/>
+      <c r="H51" s="12"/>
+      <c r="I51" s="5"/>
+    </row>
+    <row r="52" spans="2:9">
+      <c r="B52" s="4"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E52" s="12"/>
+      <c r="F52" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="G52" s="12"/>
+      <c r="H52" s="12"/>
+      <c r="I52" s="5"/>
+    </row>
+    <row r="53" spans="2:9">
+      <c r="B53" s="4"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="12"/>
+      <c r="G53" s="12"/>
+      <c r="H53" s="12"/>
+      <c r="I53" s="5"/>
+    </row>
+    <row r="54" spans="2:9">
+      <c r="B54" s="4"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
+      <c r="H54" s="12"/>
+      <c r="I54" s="5"/>
+    </row>
+    <row r="55" spans="2:9">
+      <c r="B55" s="4"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F55" s="12"/>
+      <c r="G55" s="12"/>
+      <c r="H55" s="12"/>
+      <c r="I55" s="5"/>
+    </row>
+    <row r="56" spans="2:9">
+      <c r="B56" s="4"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="12"/>
+      <c r="H56" s="12"/>
+      <c r="I56" s="5"/>
+    </row>
+    <row r="57" spans="2:9">
+      <c r="B57" s="4"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F57" s="12"/>
+      <c r="G57" s="12"/>
+      <c r="H57" s="12"/>
+      <c r="I57" s="5"/>
+    </row>
+    <row r="58" spans="2:9">
+      <c r="B58" s="4"/>
+      <c r="C58" s="12"/>
+      <c r="D58" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E58" s="12"/>
+      <c r="F58" s="12"/>
+      <c r="G58" s="12"/>
+      <c r="H58" s="12"/>
+      <c r="I58" s="5"/>
+    </row>
+    <row r="59" spans="2:9">
+      <c r="B59" s="4"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="F59" s="12"/>
+      <c r="G59" s="12"/>
+      <c r="H59" s="12"/>
+      <c r="I59" s="5"/>
+    </row>
+    <row r="60" spans="2:9">
+      <c r="B60" s="4"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="12"/>
+      <c r="H60" s="12"/>
+      <c r="I60" s="5"/>
+    </row>
+    <row r="61" spans="2:9">
+      <c r="B61" s="4"/>
+      <c r="C61" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D61" s="12"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
+      <c r="G61" s="12"/>
+      <c r="H61" s="12"/>
+      <c r="I61" s="5"/>
+    </row>
+    <row r="62" spans="2:9">
+      <c r="B62" s="4"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="12"/>
+      <c r="E62" s="12"/>
+      <c r="F62" s="12"/>
+      <c r="G62" s="12"/>
+      <c r="H62" s="12"/>
+      <c r="I62" s="5"/>
+    </row>
+    <row r="63" spans="2:9">
+      <c r="B63" s="4"/>
+      <c r="C63" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D63" s="12"/>
+      <c r="E63" s="12"/>
+      <c r="F63" s="12"/>
+      <c r="G63" s="12"/>
+      <c r="H63" s="12"/>
+      <c r="I63" s="5"/>
+    </row>
+    <row r="64" spans="2:9">
+      <c r="B64" s="4"/>
+      <c r="C64" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D64" s="12"/>
+      <c r="E64" s="12"/>
+      <c r="F64" s="12"/>
+      <c r="G64" s="12"/>
+      <c r="H64" s="12"/>
+      <c r="I64" s="5"/>
+    </row>
+    <row r="65" spans="2:9">
+      <c r="B65" s="4"/>
+      <c r="C65" s="12"/>
+      <c r="D65" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E65" s="12"/>
+      <c r="F65" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G65" s="12"/>
+      <c r="H65" s="12"/>
+      <c r="I65" s="5"/>
+    </row>
+    <row r="66" spans="2:9">
+      <c r="B66" s="4"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E66" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F66" s="12"/>
+      <c r="G66" s="12"/>
+      <c r="H66" s="12"/>
+      <c r="I66" s="5"/>
+    </row>
+    <row r="67" spans="2:9">
+      <c r="B67" s="4"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="12"/>
+      <c r="F67" s="12"/>
+      <c r="G67" s="12"/>
+      <c r="H67" s="12"/>
+      <c r="I67" s="5"/>
+    </row>
+    <row r="68" spans="2:9">
+      <c r="B68" s="4"/>
+      <c r="C68" s="12"/>
+      <c r="D68" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E68" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F68" s="12"/>
+      <c r="G68" s="12"/>
+      <c r="H68" s="12"/>
+      <c r="I68" s="5"/>
+    </row>
+    <row r="69" spans="2:9">
+      <c r="B69" s="4"/>
+      <c r="C69" s="12"/>
+      <c r="D69" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E69" s="12"/>
+      <c r="F69" s="12"/>
+      <c r="G69" s="12"/>
+      <c r="H69" s="12"/>
+      <c r="I69" s="5"/>
+    </row>
+    <row r="70" spans="2:9">
+      <c r="B70" s="4"/>
+      <c r="C70" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D70" s="12"/>
+      <c r="E70" s="12"/>
+      <c r="F70" s="12"/>
+      <c r="G70" s="12"/>
+      <c r="H70" s="12"/>
+      <c r="I70" s="5"/>
+    </row>
+    <row r="71" spans="2:9">
+      <c r="B71" s="4"/>
+      <c r="C71" s="12"/>
+      <c r="D71" s="12"/>
+      <c r="E71" s="12"/>
+      <c r="F71" s="12"/>
+      <c r="G71" s="12"/>
+      <c r="H71" s="12"/>
+      <c r="I71" s="5"/>
+    </row>
+    <row r="72" spans="2:9">
+      <c r="B72" s="4"/>
+      <c r="C72" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D72" s="12"/>
+      <c r="E72" s="12"/>
+      <c r="F72" s="12"/>
+      <c r="G72" s="12"/>
+      <c r="H72" s="12"/>
+      <c r="I72" s="5"/>
+    </row>
+    <row r="73" spans="2:9">
+      <c r="B73" s="4"/>
+      <c r="C73" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D73" s="12"/>
+      <c r="E73" s="12"/>
+      <c r="F73" s="12"/>
+      <c r="G73" s="12"/>
+      <c r="H73" s="12"/>
+      <c r="I73" s="5"/>
+    </row>
+    <row r="74" spans="2:9">
+      <c r="B74" s="4"/>
+      <c r="C74" s="12"/>
+      <c r="D74" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E74" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F74" s="12"/>
+      <c r="G74" s="12"/>
+      <c r="H74" s="12"/>
+      <c r="I74" s="5"/>
+    </row>
+    <row r="75" spans="2:9">
+      <c r="B75" s="4"/>
+      <c r="C75" s="12"/>
+      <c r="D75" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E75" s="12"/>
+      <c r="F75" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G75" s="12"/>
+      <c r="H75" s="12"/>
+      <c r="I75" s="5"/>
+    </row>
+    <row r="76" spans="2:9">
+      <c r="B76" s="4"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E76" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F76" s="12"/>
+      <c r="G76" s="12"/>
+      <c r="H76" s="12"/>
+      <c r="I76" s="5"/>
+    </row>
+    <row r="77" spans="2:9">
+      <c r="B77" s="4"/>
+      <c r="C77" s="12"/>
+      <c r="D77" s="12"/>
+      <c r="E77" s="12"/>
+      <c r="F77" s="12"/>
+      <c r="G77" s="12"/>
+      <c r="H77" s="12"/>
+      <c r="I77" s="5"/>
+    </row>
+    <row r="78" spans="2:9">
+      <c r="B78" s="4"/>
+      <c r="C78" s="12"/>
+      <c r="D78" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E78" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F78" s="12"/>
+      <c r="G78" s="12"/>
+      <c r="H78" s="12"/>
+      <c r="I78" s="5"/>
+    </row>
+    <row r="79" spans="2:9">
+      <c r="B79" s="4"/>
+      <c r="C79" s="12"/>
+      <c r="D79" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E79" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F79" s="12"/>
+      <c r="G79" s="12"/>
+      <c r="H79" s="12"/>
+      <c r="I79" s="5"/>
+    </row>
+    <row r="80" spans="2:9">
+      <c r="B80" s="4"/>
+      <c r="C80" s="12"/>
+      <c r="D80" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E80" s="12"/>
+      <c r="F80" s="12"/>
+      <c r="G80" s="12"/>
+      <c r="H80" s="12"/>
+      <c r="I80" s="5"/>
+    </row>
+    <row r="81" spans="2:9">
+      <c r="B81" s="4"/>
+      <c r="C81" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D81" s="12"/>
+      <c r="E81" s="12"/>
+      <c r="F81" s="12"/>
+      <c r="G81" s="12"/>
+      <c r="H81" s="12"/>
+      <c r="I81" s="5"/>
+    </row>
+    <row r="82" spans="2:9">
+      <c r="B82" s="4"/>
+      <c r="C82" s="12"/>
+      <c r="D82" s="12"/>
+      <c r="E82" s="12"/>
+      <c r="F82" s="12"/>
+      <c r="G82" s="12"/>
+      <c r="H82" s="12"/>
+      <c r="I82" s="5"/>
+    </row>
+    <row r="83" spans="2:9">
+      <c r="B83" s="4"/>
+      <c r="C83" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D83" s="12"/>
+      <c r="E83" s="12"/>
+      <c r="F83" s="12"/>
+      <c r="G83" s="12"/>
+      <c r="H83" s="12"/>
+      <c r="I83" s="5"/>
+    </row>
+    <row r="84" spans="2:9">
+      <c r="B84" s="4"/>
+      <c r="C84" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D84" s="12"/>
+      <c r="E84" s="12"/>
+      <c r="F84" s="12"/>
+      <c r="G84" s="12"/>
+      <c r="H84" s="12"/>
+      <c r="I84" s="5"/>
+    </row>
+    <row r="85" spans="2:9">
+      <c r="B85" s="4"/>
+      <c r="C85" s="12"/>
+      <c r="D85" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E85" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F85" s="12"/>
+      <c r="G85" s="12"/>
+      <c r="H85" s="12"/>
+      <c r="I85" s="5"/>
+    </row>
+    <row r="86" spans="2:9">
+      <c r="B86" s="4"/>
+      <c r="C86" s="12"/>
+      <c r="D86" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E86" s="12"/>
+      <c r="F86" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G86" s="12"/>
+      <c r="H86" s="12"/>
+      <c r="I86" s="5"/>
+    </row>
+    <row r="87" spans="2:9">
+      <c r="B87" s="4"/>
+      <c r="C87" s="12"/>
+      <c r="D87" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E87" s="12"/>
+      <c r="F87" s="12"/>
+      <c r="G87" s="12"/>
+      <c r="H87" s="12"/>
+      <c r="I87" s="5"/>
+    </row>
+    <row r="88" spans="2:9">
+      <c r="B88" s="4"/>
+      <c r="C88" s="12"/>
+      <c r="D88" s="12"/>
+      <c r="E88" s="12"/>
+      <c r="F88" s="12"/>
+      <c r="G88" s="12"/>
+      <c r="H88" s="12"/>
+      <c r="I88" s="5"/>
+    </row>
+    <row r="89" spans="2:9">
+      <c r="B89" s="4"/>
+      <c r="C89" s="12"/>
+      <c r="D89" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E89" s="12"/>
+      <c r="F89" s="12"/>
+      <c r="G89" s="12"/>
+      <c r="H89" s="12"/>
+      <c r="I89" s="5"/>
+    </row>
+    <row r="90" spans="2:9">
+      <c r="B90" s="4"/>
+      <c r="C90" s="12"/>
+      <c r="D90" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E90" s="12"/>
+      <c r="F90" s="12"/>
+      <c r="G90" s="12"/>
+      <c r="H90" s="12"/>
+      <c r="I90" s="5"/>
+    </row>
+    <row r="91" spans="2:9">
+      <c r="B91" s="4"/>
+      <c r="C91" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D91" s="12"/>
+      <c r="E91" s="12"/>
+      <c r="F91" s="12"/>
+      <c r="G91" s="12"/>
+      <c r="H91" s="12"/>
+      <c r="I91" s="5"/>
+    </row>
+    <row r="92" spans="2:9">
+      <c r="B92" s="4"/>
+      <c r="C92" s="12"/>
+      <c r="D92" s="12"/>
+      <c r="E92" s="12"/>
+      <c r="F92" s="12"/>
+      <c r="G92" s="12"/>
+      <c r="H92" s="12"/>
+      <c r="I92" s="5"/>
+    </row>
+    <row r="93" spans="2:9">
+      <c r="B93" s="4"/>
+      <c r="C93" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D93" s="12"/>
+      <c r="E93" s="12"/>
+      <c r="F93" s="12"/>
+      <c r="G93" s="12"/>
+      <c r="H93" s="12"/>
+      <c r="I93" s="5"/>
+    </row>
+    <row r="94" spans="2:9">
+      <c r="B94" s="4"/>
+      <c r="C94" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D94" s="12"/>
+      <c r="E94" s="12"/>
+      <c r="F94" s="12"/>
+      <c r="G94" s="12"/>
+      <c r="H94" s="12"/>
+      <c r="I94" s="5"/>
+    </row>
+    <row r="95" spans="2:9">
+      <c r="B95" s="4"/>
+      <c r="C95" s="12"/>
+      <c r="D95" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E95" s="12"/>
+      <c r="F95" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G95" s="12"/>
+      <c r="H95" s="12"/>
+      <c r="I95" s="5"/>
+    </row>
+    <row r="96" spans="2:9">
+      <c r="B96" s="4"/>
+      <c r="C96" s="12"/>
+      <c r="D96" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E96" s="12"/>
+      <c r="F96" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G96" s="12"/>
+      <c r="H96" s="12"/>
+      <c r="I96" s="5"/>
+    </row>
+    <row r="97" spans="2:9">
+      <c r="B97" s="4"/>
+      <c r="C97" s="12"/>
+      <c r="D97" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E97" s="12"/>
+      <c r="F97" s="12"/>
+      <c r="G97" s="12"/>
+      <c r="H97" s="12"/>
+      <c r="I97" s="5"/>
+    </row>
+    <row r="98" spans="2:9">
+      <c r="B98" s="4"/>
+      <c r="C98" s="12"/>
+      <c r="D98" s="12"/>
+      <c r="E98" s="12"/>
+      <c r="F98" s="12"/>
+      <c r="G98" s="12"/>
+      <c r="H98" s="12"/>
+      <c r="I98" s="5"/>
+    </row>
+    <row r="99" spans="2:9">
+      <c r="B99" s="4"/>
+      <c r="C99" s="12"/>
+      <c r="D99" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E99" s="12"/>
+      <c r="F99" s="12"/>
+      <c r="G99" s="12"/>
+      <c r="H99" s="12"/>
+      <c r="I99" s="5"/>
+    </row>
+    <row r="100" spans="2:9">
+      <c r="B100" s="4"/>
+      <c r="C100" s="12"/>
+      <c r="D100" s="12"/>
+      <c r="E100" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F100" s="12"/>
+      <c r="G100" s="12"/>
+      <c r="H100" s="12"/>
+      <c r="I100" s="5"/>
+    </row>
+    <row r="101" spans="2:9">
+      <c r="B101" s="4"/>
+      <c r="C101" s="12"/>
+      <c r="D101" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E101" s="12"/>
+      <c r="F101" s="12"/>
+      <c r="G101" s="12"/>
+      <c r="H101" s="12"/>
+      <c r="I101" s="5"/>
+    </row>
+    <row r="102" spans="2:9">
+      <c r="B102" s="4"/>
+      <c r="C102" s="12"/>
+      <c r="D102" s="12"/>
+      <c r="E102" s="12"/>
+      <c r="F102" s="12"/>
+      <c r="G102" s="12"/>
+      <c r="H102" s="12"/>
+      <c r="I102" s="5"/>
+    </row>
+    <row r="103" spans="2:9">
+      <c r="B103" s="4"/>
+      <c r="C103" s="12"/>
+      <c r="D103" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E103" s="12"/>
+      <c r="F103" s="12"/>
+      <c r="G103" s="12"/>
+      <c r="H103" s="12"/>
+      <c r="I103" s="5"/>
+    </row>
+    <row r="104" spans="2:9">
+      <c r="B104" s="4"/>
+      <c r="C104" s="12"/>
+      <c r="D104" s="12"/>
+      <c r="E104" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F104" s="12"/>
+      <c r="G104" s="12"/>
+      <c r="H104" s="12"/>
+      <c r="I104" s="5"/>
+    </row>
+    <row r="105" spans="2:9">
+      <c r="B105" s="4"/>
+      <c r="C105" s="12"/>
+      <c r="D105" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E105" s="12"/>
+      <c r="F105" s="12"/>
+      <c r="G105" s="12"/>
+      <c r="H105" s="12"/>
+      <c r="I105" s="5"/>
+    </row>
+    <row r="106" spans="2:9">
+      <c r="B106" s="4"/>
+      <c r="C106" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D106" s="12"/>
+      <c r="E106" s="12"/>
+      <c r="F106" s="12"/>
+      <c r="G106" s="12"/>
+      <c r="H106" s="12"/>
+      <c r="I106" s="5"/>
+    </row>
+    <row r="107" spans="2:9">
+      <c r="B107" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C107" s="12"/>
+      <c r="D107" s="12"/>
+      <c r="E107" s="12"/>
+      <c r="F107" s="12"/>
+      <c r="G107" s="12"/>
+      <c r="H107" s="12"/>
+      <c r="I107" s="5"/>
+    </row>
+    <row r="108" spans="2:9">
+      <c r="B108" s="7"/>
+      <c r="C108" s="8"/>
+      <c r="D108" s="8"/>
+      <c r="E108" s="8"/>
+      <c r="F108" s="8"/>
+      <c r="G108" s="8"/>
+      <c r="H108" s="8"/>
+      <c r="I108" s="9"/>
+    </row>
+    <row r="155" spans="2:13">
+      <c r="B155" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C155" s="2"/>
+      <c r="D155" s="2"/>
+      <c r="E155" s="2"/>
+      <c r="F155" s="2"/>
+      <c r="G155" s="2"/>
+      <c r="H155" s="2"/>
+      <c r="I155" s="2"/>
+      <c r="J155" s="2"/>
+      <c r="K155" s="2"/>
+      <c r="L155" s="2"/>
+      <c r="M155" s="3"/>
+    </row>
+    <row r="156" spans="2:13">
+      <c r="B156" s="4"/>
+      <c r="C156" s="12"/>
+      <c r="D156" s="12"/>
+      <c r="E156" s="12"/>
+      <c r="F156" s="12"/>
+      <c r="G156" s="12"/>
+      <c r="H156" s="12"/>
+      <c r="I156" s="12"/>
+      <c r="J156" s="12"/>
+      <c r="K156" s="12"/>
+      <c r="L156" s="12"/>
+      <c r="M156" s="5"/>
+    </row>
+    <row r="157" spans="2:13">
+      <c r="B157" s="4"/>
+      <c r="C157" s="12"/>
+      <c r="D157" s="12"/>
+      <c r="E157" s="12"/>
+      <c r="F157" s="12"/>
+      <c r="G157" s="12"/>
+      <c r="H157" s="12"/>
+      <c r="I157" s="12"/>
+      <c r="J157" s="12"/>
+      <c r="K157" s="12"/>
+      <c r="L157" s="12"/>
+      <c r="M157" s="5"/>
+    </row>
+    <row r="158" spans="2:13">
+      <c r="B158" s="4"/>
+      <c r="C158" s="12"/>
+      <c r="D158" s="12"/>
+      <c r="E158" s="12"/>
+      <c r="F158" s="12"/>
+      <c r="G158" s="12"/>
+      <c r="H158" s="12"/>
+      <c r="I158" s="12"/>
+      <c r="J158" s="12"/>
+      <c r="K158" s="12"/>
+      <c r="L158" s="12"/>
+      <c r="M158" s="5"/>
+    </row>
+    <row r="159" spans="2:13">
+      <c r="B159" s="4"/>
+      <c r="C159" s="12"/>
+      <c r="D159" s="12"/>
+      <c r="E159" s="12"/>
+      <c r="F159" s="12"/>
+      <c r="G159" s="12"/>
+      <c r="H159" s="12"/>
+      <c r="I159" s="12"/>
+      <c r="J159" s="12"/>
+      <c r="K159" s="12"/>
+      <c r="L159" s="12"/>
+      <c r="M159" s="5"/>
+    </row>
+    <row r="160" spans="2:13">
+      <c r="B160" s="4"/>
+      <c r="C160" s="12"/>
+      <c r="D160" s="12"/>
+      <c r="E160" s="12"/>
+      <c r="F160" s="12"/>
+      <c r="G160" s="12"/>
+      <c r="H160" s="12"/>
+      <c r="I160" s="12"/>
+      <c r="J160" s="12"/>
+      <c r="K160" s="12"/>
+      <c r="L160" s="12"/>
+      <c r="M160" s="5"/>
+    </row>
+    <row r="161" spans="2:13">
+      <c r="B161" s="4"/>
+      <c r="C161" s="12"/>
+      <c r="D161" s="12"/>
+      <c r="E161" s="12"/>
+      <c r="F161" s="12"/>
+      <c r="G161" s="12"/>
+      <c r="H161" s="12"/>
+      <c r="I161" s="12"/>
+      <c r="J161" s="12"/>
+      <c r="K161" s="12"/>
+      <c r="L161" s="12"/>
+      <c r="M161" s="5"/>
+    </row>
+    <row r="162" spans="2:13">
+      <c r="B162" s="4"/>
+      <c r="C162" s="12"/>
+      <c r="D162" s="12"/>
+      <c r="E162" s="12"/>
+      <c r="F162" s="12"/>
+      <c r="G162" s="12"/>
+      <c r="H162" s="12"/>
+      <c r="I162" s="12"/>
+      <c r="J162" s="12"/>
+      <c r="K162" s="12"/>
+      <c r="L162" s="12"/>
+      <c r="M162" s="5"/>
+    </row>
+    <row r="163" spans="2:13">
+      <c r="B163" s="4"/>
+      <c r="C163" s="12"/>
+      <c r="D163" s="12"/>
+      <c r="E163" s="12"/>
+      <c r="F163" s="12"/>
+      <c r="G163" s="12"/>
+      <c r="H163" s="12"/>
+      <c r="I163" s="12"/>
+      <c r="J163" s="12"/>
+      <c r="K163" s="12"/>
+      <c r="L163" s="12"/>
+      <c r="M163" s="5"/>
+    </row>
+    <row r="164" spans="2:13">
+      <c r="B164" s="4"/>
+      <c r="C164" s="12"/>
+      <c r="D164" s="12"/>
+      <c r="E164" s="12"/>
+      <c r="F164" s="12"/>
+      <c r="G164" s="12"/>
+      <c r="H164" s="12"/>
+      <c r="I164" s="12"/>
+      <c r="J164" s="12"/>
+      <c r="K164" s="12"/>
+      <c r="L164" s="12"/>
+      <c r="M164" s="5"/>
+    </row>
+    <row r="165" spans="2:13">
+      <c r="B165" s="4"/>
+      <c r="C165" s="12"/>
+      <c r="D165" s="12"/>
+      <c r="E165" s="12"/>
+      <c r="F165" s="12"/>
+      <c r="G165" s="12"/>
+      <c r="H165" s="12"/>
+      <c r="I165" s="12"/>
+      <c r="J165" s="12"/>
+      <c r="K165" s="12"/>
+      <c r="L165" s="12"/>
+      <c r="M165" s="5"/>
+    </row>
+    <row r="166" spans="2:13">
+      <c r="B166" s="4"/>
+      <c r="C166" s="12"/>
+      <c r="D166" s="12"/>
+      <c r="E166" s="12"/>
+      <c r="F166" s="12"/>
+      <c r="G166" s="12"/>
+      <c r="H166" s="12"/>
+      <c r="I166" s="12"/>
+      <c r="J166" s="12"/>
+      <c r="K166" s="12"/>
+      <c r="L166" s="12"/>
+      <c r="M166" s="5"/>
+    </row>
+    <row r="167" spans="2:13">
+      <c r="B167" s="4"/>
+      <c r="C167" s="12"/>
+      <c r="D167" s="12"/>
+      <c r="E167" s="12"/>
+      <c r="F167" s="12"/>
+      <c r="G167" s="12"/>
+      <c r="H167" s="12"/>
+      <c r="I167" s="12"/>
+      <c r="J167" s="12"/>
+      <c r="K167" s="12"/>
+      <c r="L167" s="12"/>
+      <c r="M167" s="5"/>
+    </row>
+    <row r="168" spans="2:13">
+      <c r="B168" s="4"/>
+      <c r="C168" s="12"/>
+      <c r="D168" s="12"/>
+      <c r="E168" s="12"/>
+      <c r="F168" s="12"/>
+      <c r="G168" s="12"/>
+      <c r="H168" s="12"/>
+      <c r="I168" s="12"/>
+      <c r="J168" s="12"/>
+      <c r="K168" s="12"/>
+      <c r="L168" s="12"/>
+      <c r="M168" s="5"/>
+    </row>
+    <row r="169" spans="2:13">
+      <c r="B169" s="4"/>
+      <c r="C169" s="12"/>
+      <c r="D169" s="12"/>
+      <c r="E169" s="12"/>
+      <c r="F169" s="12"/>
+      <c r="G169" s="12"/>
+      <c r="H169" s="12"/>
+      <c r="I169" s="12"/>
+      <c r="J169" s="12"/>
+      <c r="K169" s="12"/>
+      <c r="L169" s="12"/>
+      <c r="M169" s="5"/>
+    </row>
+    <row r="170" spans="2:13">
+      <c r="B170" s="4"/>
+      <c r="C170" s="12"/>
+      <c r="D170" s="12"/>
+      <c r="E170" s="12"/>
+      <c r="F170" s="12"/>
+      <c r="G170" s="12"/>
+      <c r="H170" s="12"/>
+      <c r="I170" s="12"/>
+      <c r="J170" s="12"/>
+      <c r="K170" s="12"/>
+      <c r="L170" s="12"/>
+      <c r="M170" s="5"/>
+    </row>
+    <row r="171" spans="2:13">
+      <c r="B171" s="4"/>
+      <c r="C171" s="12"/>
+      <c r="D171" s="12"/>
+      <c r="E171" s="12"/>
+      <c r="F171" s="12"/>
+      <c r="G171" s="12"/>
+      <c r="H171" s="12"/>
+      <c r="I171" s="12"/>
+      <c r="J171" s="12"/>
+      <c r="K171" s="12"/>
+      <c r="L171" s="12"/>
+      <c r="M171" s="5"/>
+    </row>
+    <row r="172" spans="2:13">
+      <c r="B172" s="4"/>
+      <c r="C172" s="12"/>
+      <c r="D172" s="12"/>
+      <c r="E172" s="12"/>
+      <c r="F172" s="12"/>
+      <c r="G172" s="12"/>
+      <c r="H172" s="12"/>
+      <c r="I172" s="12"/>
+      <c r="J172" s="12"/>
+      <c r="K172" s="12"/>
+      <c r="L172" s="12"/>
+      <c r="M172" s="5"/>
+    </row>
+    <row r="173" spans="2:13">
+      <c r="B173" s="4"/>
+      <c r="C173" s="12"/>
+      <c r="D173" s="12"/>
+      <c r="E173" s="12"/>
+      <c r="F173" s="12"/>
+      <c r="G173" s="12"/>
+      <c r="H173" s="12"/>
+      <c r="I173" s="12"/>
+      <c r="J173" s="12"/>
+      <c r="K173" s="12"/>
+      <c r="L173" s="12"/>
+      <c r="M173" s="5"/>
+    </row>
+    <row r="174" spans="2:13">
+      <c r="B174" s="7"/>
+      <c r="C174" s="8"/>
+      <c r="D174" s="8"/>
+      <c r="E174" s="8"/>
+      <c r="F174" s="8"/>
+      <c r="G174" s="8"/>
+      <c r="H174" s="8"/>
+      <c r="I174" s="8"/>
+      <c r="J174" s="8"/>
+      <c r="K174" s="8"/>
+      <c r="L174" s="8"/>
+      <c r="M174" s="9"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>